<commit_message>
updated business model zukan
ビジネスモデル図鑑を更新
</commit_message>
<xml_diff>
--- a/ビジネスモデル図鑑.xlsx
+++ b/ビジネスモデル図鑑.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\10001210862\Documents\TopSE\ソフトウェア開発実践演習\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\10001210862\Documents\TopSE\ソフトウェア開発実践演習\git\team\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="277">
   <si>
     <t>No.</t>
   </si>
@@ -1326,9 +1326,6 @@
     <t>SCOUTER</t>
   </si>
   <si>
-    <t>プロシューマ―</t>
-  </si>
-  <si>
     <t>クラウドソーシング</t>
   </si>
   <si>
@@ -1379,6 +1376,511 @@
   </si>
   <si>
     <t>Mikkeller</t>
+  </si>
+  <si>
+    <t>086</t>
+  </si>
+  <si>
+    <t>ダイアログ・イン・ザ・ダーク</t>
+  </si>
+  <si>
+    <t>体験の販売</t>
+    <rPh sb="0" eb="2">
+      <t>タイケン</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ハンバイ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>087</t>
+  </si>
+  <si>
+    <t>キッチハイク</t>
+  </si>
+  <si>
+    <t>088</t>
+  </si>
+  <si>
+    <t>WeLive</t>
+  </si>
+  <si>
+    <t>部分所有</t>
+    <rPh sb="0" eb="2">
+      <t>ブブン</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>ショユウ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>隠れた収益源</t>
+    <rPh sb="0" eb="1">
+      <t>カク</t>
+    </rPh>
+    <rPh sb="3" eb="6">
+      <t>シュウエキゲン</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>089</t>
+  </si>
+  <si>
+    <t>LifeStraw</t>
+  </si>
+  <si>
+    <t>押収した違法銃</t>
+    <rPh sb="0" eb="2">
+      <t>オウシュウ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>イホウ</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>ジュウ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>処分できずに放置</t>
+    <rPh sb="0" eb="2">
+      <t>ショブン</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>ホウチ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>処分させずに収益化</t>
+    <rPh sb="0" eb="2">
+      <t>ショブン</t>
+    </rPh>
+    <rPh sb="6" eb="9">
+      <t>シュウエキカ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>違法な銃がおしゃれな時計や自転車に変わる</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>「公共事業はお金がかかる」を覆す、すごい仕組み</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>公共事業</t>
+    <rPh sb="0" eb="2">
+      <t>コウキョウ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>ジギョウ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>成果にかかわらず費用がかかる</t>
+    <rPh sb="0" eb="2">
+      <t>セイカ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>ヒヨウ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>成果に合わせて費用がかかる</t>
+    <rPh sb="0" eb="2">
+      <t>セイカ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>ア</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>ヒヨウ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>「友人・知人のネットワーク」を活用した転職エージェント</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>転職エージェント</t>
+    <rPh sb="0" eb="2">
+      <t>テンショク</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>プロが専業でやるもの</t>
+    <rPh sb="3" eb="5">
+      <t>センギョウ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>個人が副業でやるもの</t>
+    <rPh sb="0" eb="2">
+      <t>コジン</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>フクギョウ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>ファンの間で熱狂的な人気を誇る「クソアニメ」</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>深夜アニメ</t>
+    <rPh sb="0" eb="2">
+      <t>シンヤ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>制作委員会方式が主流</t>
+    <rPh sb="0" eb="2">
+      <t>セイサク</t>
+    </rPh>
+    <rPh sb="2" eb="5">
+      <t>イインカイ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>ホウシキ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>シュリュウ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>単独出資方式で制作</t>
+    <rPh sb="0" eb="2">
+      <t>タンドク</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>シュッシ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>ホウシキ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>セイサク</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>人だけでなくモノも運ぶ「インドネシア版Uber」</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>バイクタクシー</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>交通インフラ</t>
+    <rPh sb="0" eb="2">
+      <t>コウツウ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>物流インフラ</t>
+    <rPh sb="0" eb="2">
+      <t>ブツリュウ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>ホームレスの自立を応援するための雑誌</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>ホームレス支援</t>
+    <rPh sb="5" eb="7">
+      <t>シエン</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>寄付や物品による支援</t>
+    <rPh sb="0" eb="2">
+      <t>キフ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ブッピン</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>シエン</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>自立を促すための仕事の提供による支援</t>
+    <rPh sb="0" eb="2">
+      <t>ジリツ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>ウナガ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>シゴト</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>テイキョウ</t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t>シエン</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>ミクシィがはじめたサロンスタッフを「直接指名」できるアプリ</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>美容系マッチングアプリ</t>
+    <rPh sb="0" eb="2">
+      <t>ビヨウ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>ケイ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>スタッフではなくサロンを探すもの</t>
+    <rPh sb="12" eb="13">
+      <t>サガ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>サロンではなくスタッフを探すもの</t>
+    <rPh sb="12" eb="13">
+      <t>サガ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>年間100種類の新商品を生み出す「設備を持たない」ビールメーカー</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>クラフトビール製造</t>
+    <rPh sb="7" eb="9">
+      <t>セイゾウ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>自社の設備でつくるもの</t>
+    <rPh sb="0" eb="2">
+      <t>ジシャ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>セツビ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>他社の設備でつくるもの</t>
+    <rPh sb="0" eb="2">
+      <t>タシャ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>セツビ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>完全暗闇を体感するソーシャルエンターテインメント</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>体験型ワークショップ</t>
+    <rPh sb="0" eb="3">
+      <t>タイケンガタ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>すべての感覚を使って体験する</t>
+    <rPh sb="4" eb="6">
+      <t>カンカク</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>ツカ</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>タイケン</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>視覚以外の感覚を使って体験する</t>
+    <rPh sb="0" eb="2">
+      <t>シカク</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>イガイ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>カンカク</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>ツカ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>タイケン</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>料理を「つくりたい人」と「食べたい人」をつなぐコミュニティ</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>手作り料理</t>
+    <rPh sb="0" eb="2">
+      <t>テヅク</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>リョウリ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>家族や友人にふるまうもの</t>
+    <rPh sb="0" eb="2">
+      <t>カゾク</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ユウジン</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>初めての人にもふるまえるもの</t>
+    <rPh sb="0" eb="1">
+      <t>ハジ</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>ヒト</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>「WeWork」（シェアオフィス）に続く、コミュニティ重視の居住スタイル</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>シェアハウス</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>コミュニティマネージャーがいない</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>コミュニティマネージャーがいる</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>安全な水が飲めるストロー型の浄水器</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>困りごとを解決する商品</t>
+    <rPh sb="0" eb="1">
+      <t>コマ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>カイケツ</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>ショウヒン</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>必要とする人が対価を払う</t>
+    <rPh sb="0" eb="2">
+      <t>ヒツヨウ</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>ヒト</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>タイカ</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>ハラ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>社会課題に関心のある企業が対価を払う</t>
+    <rPh sb="0" eb="2">
+      <t>シャカイ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>カダイ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>カンシン</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>キギョウ</t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t>タイカ</t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t>ハラ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>業界をアシストする</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>隠れた収益源</t>
+    <rPh sb="0" eb="1">
+      <t>カク</t>
+    </rPh>
+    <rPh sb="3" eb="6">
+      <t>シュウエキゲン</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>ライセンシング</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>クラウドソーシング</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>プロシューマ―</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>クロスセル</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>オーケストレーター</t>
+    <phoneticPr fontId="4"/>
   </si>
   <si>
     <t>OEM製品</t>
@@ -1388,492 +1890,18 @@
     <phoneticPr fontId="4"/>
   </si>
   <si>
-    <t>086</t>
-  </si>
-  <si>
-    <t>ダイアログ・イン・ザ・ダーク</t>
-  </si>
-  <si>
-    <t>体験の販売</t>
-    <rPh sb="0" eb="2">
-      <t>タイケン</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>ハンバイ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>087</t>
-  </si>
-  <si>
-    <t>キッチハイク</t>
-  </si>
-  <si>
-    <t>088</t>
-  </si>
-  <si>
-    <t>WeLive</t>
-  </si>
-  <si>
-    <t>部分所有</t>
-    <rPh sb="0" eb="2">
-      <t>ブブン</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>ショユウ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>隠れた収益源</t>
-    <rPh sb="0" eb="1">
-      <t>カク</t>
-    </rPh>
-    <rPh sb="3" eb="6">
-      <t>シュウエキゲン</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>089</t>
-  </si>
-  <si>
-    <t>LifeStraw</t>
-  </si>
-  <si>
-    <t>押収した違法銃</t>
-    <rPh sb="0" eb="2">
-      <t>オウシュウ</t>
-    </rPh>
-    <rPh sb="4" eb="6">
-      <t>イホウ</t>
-    </rPh>
-    <rPh sb="6" eb="7">
-      <t>ジュウ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>処分できずに放置</t>
-    <rPh sb="0" eb="2">
-      <t>ショブン</t>
-    </rPh>
-    <rPh sb="6" eb="8">
-      <t>ホウチ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>処分させずに収益化</t>
-    <rPh sb="0" eb="2">
-      <t>ショブン</t>
-    </rPh>
-    <rPh sb="6" eb="9">
-      <t>シュウエキカ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>違法な銃がおしゃれな時計や自転車に変わる</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>「公共事業はお金がかかる」を覆す、すごい仕組み</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>公共事業</t>
-    <rPh sb="0" eb="2">
-      <t>コウキョウ</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>ジギョウ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>成果にかかわらず費用がかかる</t>
-    <rPh sb="0" eb="2">
-      <t>セイカ</t>
-    </rPh>
-    <rPh sb="8" eb="10">
-      <t>ヒヨウ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>成果に合わせて費用がかかる</t>
-    <rPh sb="0" eb="2">
-      <t>セイカ</t>
-    </rPh>
-    <rPh sb="3" eb="4">
-      <t>ア</t>
-    </rPh>
-    <rPh sb="7" eb="9">
-      <t>ヒヨウ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>「友人・知人のネットワーク」を活用した転職エージェント</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>転職エージェント</t>
-    <rPh sb="0" eb="2">
-      <t>テンショク</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>プロが専業でやるもの</t>
-    <rPh sb="3" eb="5">
-      <t>センギョウ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>個人が副業でやるもの</t>
-    <rPh sb="0" eb="2">
-      <t>コジン</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>フクギョウ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>ファンの間で熱狂的な人気を誇る「クソアニメ」</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>深夜アニメ</t>
-    <rPh sb="0" eb="2">
-      <t>シンヤ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>制作委員会方式が主流</t>
-    <rPh sb="0" eb="2">
-      <t>セイサク</t>
-    </rPh>
-    <rPh sb="2" eb="5">
-      <t>イインカイ</t>
-    </rPh>
-    <rPh sb="5" eb="7">
-      <t>ホウシキ</t>
-    </rPh>
-    <rPh sb="8" eb="10">
-      <t>シュリュウ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>単独出資方式で制作</t>
-    <rPh sb="0" eb="2">
-      <t>タンドク</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>シュッシ</t>
-    </rPh>
-    <rPh sb="4" eb="6">
-      <t>ホウシキ</t>
-    </rPh>
-    <rPh sb="7" eb="9">
-      <t>セイサク</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>人だけでなくモノも運ぶ「インドネシア版Uber」</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>バイクタクシー</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>交通インフラ</t>
-    <rPh sb="0" eb="2">
-      <t>コウツウ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>物流インフラ</t>
-    <rPh sb="0" eb="2">
-      <t>ブツリュウ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>ホームレスの自立を応援するための雑誌</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>ホームレス支援</t>
-    <rPh sb="5" eb="7">
-      <t>シエン</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>寄付や物品による支援</t>
-    <rPh sb="0" eb="2">
-      <t>キフ</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>ブッピン</t>
-    </rPh>
-    <rPh sb="8" eb="10">
-      <t>シエン</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>自立を促すための仕事の提供による支援</t>
-    <rPh sb="0" eb="2">
-      <t>ジリツ</t>
-    </rPh>
-    <rPh sb="3" eb="4">
-      <t>ウナガ</t>
-    </rPh>
-    <rPh sb="8" eb="10">
-      <t>シゴト</t>
-    </rPh>
-    <rPh sb="11" eb="13">
-      <t>テイキョウ</t>
-    </rPh>
-    <rPh sb="16" eb="18">
-      <t>シエン</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>ミクシィがはじめたサロンスタッフを「直接指名」できるアプリ</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>美容系マッチングアプリ</t>
-    <rPh sb="0" eb="2">
-      <t>ビヨウ</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>ケイ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>スタッフではなくサロンを探すもの</t>
-    <rPh sb="12" eb="13">
-      <t>サガ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>サロンではなくスタッフを探すもの</t>
-    <rPh sb="12" eb="13">
-      <t>サガ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>年間100種類の新商品を生み出す「設備を持たない」ビールメーカー</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>クラフトビール製造</t>
-    <rPh sb="7" eb="9">
-      <t>セイゾウ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>自社の設備でつくるもの</t>
-    <rPh sb="0" eb="2">
-      <t>ジシャ</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>セツビ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>他社の設備でつくるもの</t>
-    <rPh sb="0" eb="2">
-      <t>タシャ</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>セツビ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>完全暗闇を体感するソーシャルエンターテインメント</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>体験型ワークショップ</t>
-    <rPh sb="0" eb="3">
-      <t>タイケンガタ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>すべての感覚を使って体験する</t>
-    <rPh sb="4" eb="6">
-      <t>カンカク</t>
-    </rPh>
-    <rPh sb="7" eb="8">
-      <t>ツカ</t>
-    </rPh>
-    <rPh sb="10" eb="12">
-      <t>タイケン</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>視覚以外の感覚を使って体験する</t>
-    <rPh sb="0" eb="2">
-      <t>シカク</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>イガイ</t>
-    </rPh>
-    <rPh sb="5" eb="7">
-      <t>カンカク</t>
-    </rPh>
-    <rPh sb="8" eb="9">
-      <t>ツカ</t>
-    </rPh>
-    <rPh sb="11" eb="13">
-      <t>タイケン</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>料理を「つくりたい人」と「食べたい人」をつなぐコミュニティ</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>手作り料理</t>
-    <rPh sb="0" eb="2">
-      <t>テヅク</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>リョウリ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>家族や友人にふるまうもの</t>
-    <rPh sb="0" eb="2">
-      <t>カゾク</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>ユウジン</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>初めての人にもふるまえるもの</t>
-    <rPh sb="0" eb="1">
-      <t>ハジ</t>
-    </rPh>
+    <t>プロシューマ―</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>デジタル化</t>
     <rPh sb="4" eb="5">
-      <t>ヒト</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>「WeWork」（シェアオフィス）に続く、コミュニティ重視の居住スタイル</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>シェアハウス</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>コミュニティマネージャーがいない</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>コミュニティマネージャーがいる</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>安全な水が飲めるストロー型の浄水器</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>困りごとを解決する商品</t>
-    <rPh sb="0" eb="1">
-      <t>コマ</t>
-    </rPh>
-    <rPh sb="5" eb="7">
-      <t>カイケツ</t>
-    </rPh>
-    <rPh sb="9" eb="11">
-      <t>ショウヒン</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>必要とする人が対価を払う</t>
-    <rPh sb="0" eb="2">
-      <t>ヒツヨウ</t>
-    </rPh>
-    <rPh sb="5" eb="6">
-      <t>ヒト</t>
-    </rPh>
-    <rPh sb="7" eb="9">
-      <t>タイカ</t>
-    </rPh>
-    <rPh sb="10" eb="11">
-      <t>ハラ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>社会課題に関心のある企業が対価を払う</t>
-    <rPh sb="0" eb="2">
-      <t>シャカイ</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>カダイ</t>
-    </rPh>
-    <rPh sb="5" eb="7">
-      <t>カンシン</t>
-    </rPh>
-    <rPh sb="10" eb="12">
-      <t>キギョウ</t>
-    </rPh>
-    <rPh sb="13" eb="15">
-      <t>タイカ</t>
-    </rPh>
-    <rPh sb="16" eb="17">
-      <t>ハラ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>業界をアシストする</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>隠れた収益源</t>
-    <rPh sb="0" eb="1">
-      <t>カク</t>
-    </rPh>
-    <rPh sb="3" eb="6">
-      <t>シュウエキゲン</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>ライセンシング</t>
+      <t>カ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>成果報酬型契約</t>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
@@ -2302,7 +2330,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E40" sqref="E40"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="19.8"/>
@@ -2982,7 +3010,7 @@
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>137</v>
@@ -3074,20 +3102,24 @@
       <c r="D26" s="11" t="s">
         <v>187</v>
       </c>
-      <c r="E26" s="11"/>
+      <c r="E26" s="11" t="s">
+        <v>202</v>
+      </c>
       <c r="F26" s="11"/>
-      <c r="G26" s="11"/>
+      <c r="G26" s="11" t="s">
+        <v>49</v>
+      </c>
       <c r="H26" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="I26" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="J26" s="11" t="s">
         <v>220</v>
       </c>
-      <c r="I26" s="11" t="s">
+      <c r="K26" s="10" t="s">
         <v>221</v>
-      </c>
-      <c r="J26" s="11" t="s">
-        <v>222</v>
-      </c>
-      <c r="K26" s="10" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="27" spans="1:11">
@@ -3107,16 +3139,16 @@
         <v>37</v>
       </c>
       <c r="H27" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="I27" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="J27" s="11" t="s">
         <v>225</v>
       </c>
-      <c r="I27" s="11" t="s">
-        <v>226</v>
-      </c>
-      <c r="J27" s="11" t="s">
-        <v>227</v>
-      </c>
       <c r="K27" s="11" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -3127,105 +3159,111 @@
         <v>192</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>193</v>
+        <v>269</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="E28" s="11"/>
+        <v>276</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>270</v>
+      </c>
       <c r="F28" s="11"/>
       <c r="G28" s="11" t="s">
         <v>37</v>
       </c>
       <c r="H28" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="I28" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="J28" s="11" t="s">
         <v>229</v>
       </c>
-      <c r="I28" s="11" t="s">
-        <v>230</v>
-      </c>
-      <c r="J28" s="11" t="s">
-        <v>231</v>
-      </c>
       <c r="K28" s="11" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="29" spans="1:11">
       <c r="A29" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="B29" s="11" t="s">
         <v>195</v>
       </c>
-      <c r="B29" s="11" t="s">
+      <c r="C29" s="11" t="s">
         <v>196</v>
       </c>
-      <c r="C29" s="11" t="s">
-        <v>197</v>
-      </c>
       <c r="D29" s="11" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F29" s="11"/>
       <c r="G29" s="11" t="s">
         <v>38</v>
       </c>
       <c r="H29" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="I29" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="J29" s="11" t="s">
         <v>233</v>
       </c>
-      <c r="I29" s="11" t="s">
-        <v>234</v>
-      </c>
-      <c r="J29" s="11" t="s">
-        <v>235</v>
-      </c>
       <c r="K29" s="11" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="30" spans="1:11">
       <c r="A30" s="12" t="s">
+        <v>197</v>
+      </c>
+      <c r="B30" s="11" t="s">
         <v>198</v>
       </c>
-      <c r="B30" s="11" t="s">
+      <c r="C30" s="13" t="s">
         <v>199</v>
       </c>
-      <c r="C30" s="13" t="s">
-        <v>200</v>
-      </c>
       <c r="D30" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
+        <v>193</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>271</v>
+      </c>
+      <c r="F30" s="11" t="s">
+        <v>275</v>
+      </c>
       <c r="G30" t="s">
         <v>42</v>
       </c>
       <c r="H30" s="11" t="s">
+        <v>235</v>
+      </c>
+      <c r="I30" s="11" t="s">
+        <v>236</v>
+      </c>
+      <c r="J30" s="11" t="s">
         <v>237</v>
       </c>
-      <c r="I30" s="11" t="s">
-        <v>238</v>
-      </c>
-      <c r="J30" s="11" t="s">
-        <v>239</v>
-      </c>
       <c r="K30" s="11" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="31" spans="1:11">
       <c r="A31" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="B31" s="11" t="s">
         <v>201</v>
       </c>
-      <c r="B31" s="11" t="s">
+      <c r="C31" s="11" t="s">
         <v>202</v>
       </c>
-      <c r="C31" s="11" t="s">
-        <v>203</v>
-      </c>
       <c r="D31" s="11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E31" s="11"/>
       <c r="F31" s="11"/>
@@ -3233,184 +3271,208 @@
         <v>49</v>
       </c>
       <c r="H31" s="11" t="s">
+        <v>239</v>
+      </c>
+      <c r="I31" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="J31" s="11" t="s">
         <v>241</v>
       </c>
-      <c r="I31" s="11" t="s">
-        <v>242</v>
-      </c>
-      <c r="J31" s="11" t="s">
-        <v>243</v>
-      </c>
       <c r="K31" s="11" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="32" spans="1:11">
       <c r="A32" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="B32" s="11" t="s">
         <v>204</v>
       </c>
-      <c r="B32" s="11" t="s">
-        <v>205</v>
-      </c>
       <c r="C32" s="13" t="s">
-        <v>200</v>
-      </c>
-      <c r="D32" s="11"/>
+        <v>199</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>275</v>
+      </c>
       <c r="E32" s="11"/>
       <c r="F32" s="11"/>
-      <c r="G32" s="11"/>
+      <c r="G32" s="11" t="s">
+        <v>37</v>
+      </c>
       <c r="H32" s="11" t="s">
+        <v>243</v>
+      </c>
+      <c r="I32" s="11" t="s">
+        <v>244</v>
+      </c>
+      <c r="J32" s="11" t="s">
         <v>245</v>
       </c>
-      <c r="I32" s="11" t="s">
-        <v>246</v>
-      </c>
-      <c r="J32" s="11" t="s">
-        <v>247</v>
-      </c>
       <c r="K32" s="11" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="33" spans="1:11">
       <c r="A33" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="B33" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="B33" s="11" t="s">
-        <v>207</v>
-      </c>
       <c r="C33" s="11" t="s">
-        <v>208</v>
-      </c>
-      <c r="D33" s="11"/>
+        <v>272</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>273</v>
+      </c>
       <c r="E33" s="11"/>
       <c r="F33" s="11"/>
-      <c r="G33" s="11"/>
+      <c r="G33" t="s">
+        <v>38</v>
+      </c>
       <c r="H33" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="I33" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="J33" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="I33" s="11" t="s">
-        <v>250</v>
-      </c>
-      <c r="J33" s="11" t="s">
-        <v>251</v>
-      </c>
       <c r="K33" s="11" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="34" spans="1:11">
       <c r="A34" s="12" t="s">
+        <v>207</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="C34" s="11" t="s">
         <v>209</v>
-      </c>
-      <c r="B34" s="11" t="s">
-        <v>210</v>
-      </c>
-      <c r="C34" s="11" t="s">
-        <v>211</v>
       </c>
       <c r="D34" s="11"/>
       <c r="E34" s="11"/>
       <c r="F34" s="11"/>
-      <c r="G34" s="11"/>
+      <c r="G34" s="11" t="s">
+        <v>49</v>
+      </c>
       <c r="H34" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="I34" s="11" t="s">
+        <v>252</v>
+      </c>
+      <c r="J34" s="11" t="s">
         <v>253</v>
       </c>
-      <c r="I34" s="11" t="s">
-        <v>254</v>
-      </c>
-      <c r="J34" s="11" t="s">
-        <v>255</v>
-      </c>
       <c r="K34" s="11" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="35" spans="1:11">
       <c r="A35" s="12" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>193</v>
-      </c>
-      <c r="D35" s="13" t="s">
-        <v>200</v>
-      </c>
-      <c r="E35" s="11"/>
-      <c r="F35" s="11"/>
-      <c r="G35" s="11"/>
+        <v>32</v>
+      </c>
+      <c r="D35" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="E35" s="11" t="s">
+        <v>274</v>
+      </c>
+      <c r="F35" s="11" t="s">
+        <v>275</v>
+      </c>
+      <c r="G35" s="11" t="s">
+        <v>42</v>
+      </c>
       <c r="H35" s="11" t="s">
+        <v>255</v>
+      </c>
+      <c r="I35" s="11" t="s">
+        <v>256</v>
+      </c>
+      <c r="J35" s="11" t="s">
         <v>257</v>
       </c>
-      <c r="I35" s="11" t="s">
-        <v>258</v>
-      </c>
-      <c r="J35" s="11" t="s">
-        <v>259</v>
-      </c>
       <c r="K35" s="11" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="36" spans="1:11">
       <c r="A36" s="12" t="s">
+        <v>212</v>
+      </c>
+      <c r="B36" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="C36" s="11" t="s">
         <v>214</v>
       </c>
-      <c r="B36" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="C36" s="11" t="s">
-        <v>216</v>
-      </c>
       <c r="D36" s="11" t="s">
-        <v>217</v>
-      </c>
-      <c r="E36" s="11"/>
-      <c r="F36" s="11"/>
-      <c r="G36" s="11"/>
+        <v>209</v>
+      </c>
+      <c r="E36" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="F36" s="11" t="s">
+        <v>275</v>
+      </c>
+      <c r="G36" s="11" t="s">
+        <v>42</v>
+      </c>
       <c r="H36" s="11" t="s">
+        <v>259</v>
+      </c>
+      <c r="I36" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="J36" s="11" t="s">
         <v>261</v>
       </c>
-      <c r="I36" s="11" t="s">
-        <v>262</v>
-      </c>
-      <c r="J36" s="11" t="s">
-        <v>263</v>
-      </c>
       <c r="K36" s="11" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="37" spans="1:11">
       <c r="A37" s="12" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>203</v>
-      </c>
-      <c r="D37" s="11"/>
+        <v>202</v>
+      </c>
+      <c r="D37" s="11" t="s">
+        <v>215</v>
+      </c>
       <c r="E37" s="11"/>
       <c r="F37" s="11"/>
       <c r="G37" s="11" t="s">
         <v>49</v>
       </c>
       <c r="H37" s="11" t="s">
+        <v>263</v>
+      </c>
+      <c r="I37" s="11" t="s">
+        <v>264</v>
+      </c>
+      <c r="J37" s="11" t="s">
         <v>265</v>
       </c>
-      <c r="I37" s="11" t="s">
-        <v>266</v>
-      </c>
-      <c r="J37" s="11" t="s">
-        <v>267</v>
-      </c>
       <c r="K37" s="11" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="39" spans="1:11">

</xml_diff>